<commit_message>
Refactor tag dict para cambio de tipo de datos de los campos Codificación nodos etapa de procesamiento re nombrado y cambio de tipado Ajuste notebook pruebas para validar funcionalidad de nodos
</commit_message>
<xml_diff>
--- a/data/raw/tag_dict_tc.xlsx
+++ b/data/raw/tag_dict_tc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agomezj/Desktop/Data Science/Proyectos/proyecto_TC/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F920970C-83AD-CC42-BC4B-91D9360D484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90C667EF-11B6-2A44-A3B3-10645DC0A48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32220" yWindow="-920" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tag_dict" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="72">
   <si>
     <t>tag</t>
   </si>
@@ -52,212 +52,206 @@
     <t>id_cliente</t>
   </si>
   <si>
+    <t>Int64</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>edad</t>
+  </si>
+  <si>
+    <t>Tipo_Trabajo</t>
+  </si>
+  <si>
+    <t>tipo_trabajo</t>
+  </si>
+  <si>
+    <t>Estado_Civil</t>
+  </si>
+  <si>
+    <t>estado_civil</t>
+  </si>
+  <si>
+    <t>Educacion</t>
+  </si>
+  <si>
+    <t>educacion</t>
+  </si>
+  <si>
+    <t>mora</t>
+  </si>
+  <si>
+    <t>Vivienda</t>
+  </si>
+  <si>
+    <t>posee_vivienda</t>
+  </si>
+  <si>
+    <t>Vehiculo</t>
+  </si>
+  <si>
+    <t>posee_vehiculo</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>tipo_contacto</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>mes_contacto</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>dia_contacto</t>
+  </si>
+  <si>
+    <t>Campana</t>
+  </si>
+  <si>
+    <t>campania</t>
+  </si>
+  <si>
+    <t>Dias_Ultima_Camp</t>
+  </si>
+  <si>
+    <t>dias_ultima_camp</t>
+  </si>
+  <si>
+    <t>No_Contactos</t>
+  </si>
+  <si>
+    <t>nro_contactos</t>
+  </si>
+  <si>
+    <t>Resultado_Anterior</t>
+  </si>
+  <si>
+    <t>resultado_anterior</t>
+  </si>
+  <si>
+    <t>emp_var_rate</t>
+  </si>
+  <si>
+    <t>var_negocio_1</t>
+  </si>
+  <si>
+    <t>Float64</t>
+  </si>
+  <si>
+    <t>cons_price_idx</t>
+  </si>
+  <si>
+    <t>var_negocio_2</t>
+  </si>
+  <si>
+    <t>cons_conf_idx</t>
+  </si>
+  <si>
+    <t>var_negocio_3</t>
+  </si>
+  <si>
+    <t>euribor3m</t>
+  </si>
+  <si>
+    <t>var_negocio_4</t>
+  </si>
+  <si>
+    <t>nr_employed</t>
+  </si>
+  <si>
+    <t>var_negocio_5</t>
+  </si>
+  <si>
+    <t>vlr_ingresos</t>
+  </si>
+  <si>
+    <t>segmento</t>
+  </si>
+  <si>
+    <t>perfil_riesgo</t>
+  </si>
+  <si>
+    <t>marg_cont</t>
+  </si>
+  <si>
+    <t>score_cliente</t>
+  </si>
+  <si>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>cdt</t>
+  </si>
+  <si>
+    <t>sum_saldo_prom_ah</t>
+  </si>
+  <si>
+    <t>sum_monto_trx_ah</t>
+  </si>
+  <si>
+    <t>sum_cant_trx_ah</t>
+  </si>
+  <si>
+    <t>sum_saldo_prom_cc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_monto_trx_cc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_cant_trx_cc </t>
+  </si>
+  <si>
+    <t>cdt_sum_valor_interes</t>
+  </si>
+  <si>
+    <t>cdt_sum_monto_apertura</t>
+  </si>
+  <si>
+    <t>cdt_prom_plazo_total_meses</t>
+  </si>
+  <si>
+    <t>buro_max_deuda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buro_num_creditos </t>
+  </si>
+  <si>
     <t>int64</t>
   </si>
   <si>
     <t>object</t>
   </si>
   <si>
-    <t>raw</t>
-  </si>
-  <si>
-    <t>Edad</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>Tipo_Trabajo</t>
-  </si>
-  <si>
-    <t>tipo_trabajo</t>
-  </si>
-  <si>
-    <t>Estado_Civil</t>
-  </si>
-  <si>
-    <t>estado_civil</t>
-  </si>
-  <si>
-    <t>Educacion</t>
-  </si>
-  <si>
-    <t>educacion</t>
-  </si>
-  <si>
-    <t>mora</t>
-  </si>
-  <si>
-    <t>Vivienda</t>
-  </si>
-  <si>
-    <t>posee_vivienda</t>
-  </si>
-  <si>
-    <t>Vehiculo</t>
-  </si>
-  <si>
-    <t>posee_vehiculo</t>
-  </si>
-  <si>
-    <t>Contacto</t>
-  </si>
-  <si>
-    <t>tipo_contacto</t>
-  </si>
-  <si>
-    <t>Mes</t>
-  </si>
-  <si>
-    <t>mes_contacto</t>
-  </si>
-  <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>dia_contacto</t>
-  </si>
-  <si>
-    <t>Campana</t>
-  </si>
-  <si>
-    <t>campania</t>
-  </si>
-  <si>
-    <t>Dias_Ultima_Camp</t>
-  </si>
-  <si>
-    <t>dias_ultima_camp</t>
-  </si>
-  <si>
-    <t>No_Contactos</t>
-  </si>
-  <si>
-    <t>nro_contactos</t>
-  </si>
-  <si>
-    <t>Resultado_Anterior</t>
-  </si>
-  <si>
-    <t>resultado_anterior</t>
-  </si>
-  <si>
-    <t>emp_var_rate</t>
-  </si>
-  <si>
-    <t>var_negocio_1</t>
+    <t>Consumo</t>
   </si>
   <si>
     <t>float64</t>
   </si>
   <si>
-    <t>cons_price_idx</t>
-  </si>
-  <si>
-    <t>var_negocio_2</t>
-  </si>
-  <si>
-    <t>cons_conf_idx</t>
-  </si>
-  <si>
-    <t>var_negocio_3</t>
-  </si>
-  <si>
-    <t>euribor3m</t>
-  </si>
-  <si>
-    <t>var_negocio_4</t>
-  </si>
-  <si>
-    <t>nr_employed</t>
-  </si>
-  <si>
-    <t>var_negocio_5</t>
-  </si>
-  <si>
-    <t>vlr_ingresos</t>
-  </si>
-  <si>
-    <t>segmento</t>
-  </si>
-  <si>
-    <t>perfil_riesgo</t>
-  </si>
-  <si>
-    <t>marg_cont</t>
-  </si>
-  <si>
-    <t>score_cliente</t>
-  </si>
-  <si>
-    <t>ah</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>cdt</t>
-  </si>
-  <si>
-    <t>sum_saldo_prom_ah</t>
-  </si>
-  <si>
-    <t>sum_monto_trx_ah</t>
-  </si>
-  <si>
-    <t>sum_cant_trx_ah</t>
-  </si>
-  <si>
-    <t>sum_saldo_prom_cc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_monto_trx_cc </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_cant_trx_cc </t>
-  </si>
-  <si>
-    <t>cdt_sum_valor_interes</t>
-  </si>
-  <si>
-    <t>cdt_sum_monto_apertura</t>
-  </si>
-  <si>
-    <t>cdt_prom_plazo_total_meses</t>
-  </si>
-  <si>
-    <t>buro_max_deuda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buro_num_creditos </t>
-  </si>
-  <si>
-    <t>Consumo</t>
-  </si>
-  <si>
     <t>buro_num_creditos</t>
   </si>
   <si>
-    <t>Int64</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Int64</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> String</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Float64</t>
-  </si>
-  <si>
-    <t>string</t>
+    <t>String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,17 +263,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -325,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -334,6 +331,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +550,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -588,659 +586,659 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>73</v>
+      <c r="C4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>73</v>
+      <c r="C5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>73</v>
+      <c r="C6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>73</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>73</v>
+      <c r="C8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>73</v>
+      <c r="C9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>73</v>
+      <c r="C10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>73</v>
+      <c r="C11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>73</v>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>73</v>
+      <c r="C16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>73</v>
+        <v>52</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>73</v>
+        <v>54</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1269,311 +1267,311 @@
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat etapa seleccion del mejor modelo completada.
</commit_message>
<xml_diff>
--- a/data/raw/tag_dict_tc.xlsx
+++ b/data/raw/tag_dict_tc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agomezj/Desktop/Data Science/Proyectos/proyecto_TC/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agomezj/Desktop/Data Science/Proyectos/proyecto_tc/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90C667EF-11B6-2A44-A3B3-10645DC0A48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F134BE1-5F58-F344-992D-ACB86A579927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32220" yWindow="-920" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="71">
   <si>
     <t>tag</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>buro_num_creditos</t>
-  </si>
-  <si>
-    <t>String</t>
   </si>
 </sst>
 </file>
@@ -589,7 +586,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -605,8 +602,8 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
+      <c r="D3" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -620,10 +617,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -637,10 +634,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
@@ -654,10 +651,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
@@ -671,10 +668,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
@@ -688,10 +685,10 @@
         <v>19</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
@@ -705,10 +702,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>8</v>
@@ -722,10 +719,10 @@
         <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
@@ -739,10 +736,10 @@
         <v>25</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>8</v>
@@ -756,10 +753,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>8</v>
@@ -776,7 +773,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>8</v>
@@ -792,8 +789,8 @@
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
+      <c r="D14" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>8</v>
@@ -809,8 +806,8 @@
       <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
+      <c r="D15" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>8</v>
@@ -824,10 +821,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>8</v>
@@ -843,8 +840,8 @@
       <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>38</v>
+      <c r="D17" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>8</v>
@@ -860,8 +857,8 @@
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
+      <c r="D18" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>8</v>
@@ -877,8 +874,8 @@
       <c r="C19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>38</v>
+      <c r="D19" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
@@ -894,8 +891,8 @@
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
+      <c r="D20" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>8</v>
@@ -911,8 +908,8 @@
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
+      <c r="D21" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>8</v>
@@ -928,8 +925,8 @@
       <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>38</v>
+      <c r="D22" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>8</v>
@@ -943,10 +940,10 @@
         <v>48</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>8</v>
@@ -962,8 +959,8 @@
       <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
+      <c r="D24" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>8</v>
@@ -979,8 +976,8 @@
       <c r="C25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>38</v>
+      <c r="D25" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>8</v>
@@ -996,8 +993,8 @@
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>7</v>
+      <c r="D26" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>8</v>
@@ -1011,10 +1008,10 @@
         <v>52</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>8</v>
@@ -1028,10 +1025,10 @@
         <v>53</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>8</v>
@@ -1045,10 +1042,10 @@
         <v>54</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>8</v>
@@ -1064,8 +1061,8 @@
       <c r="C30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>38</v>
+      <c r="D30" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>8</v>
@@ -1081,8 +1078,8 @@
       <c r="C31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>38</v>
+      <c r="D31" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>8</v>
@@ -1098,8 +1095,8 @@
       <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>7</v>
+      <c r="D32" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>8</v>
@@ -1115,8 +1112,8 @@
       <c r="C33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>38</v>
+      <c r="D33" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>8</v>
@@ -1132,8 +1129,8 @@
       <c r="C34" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>38</v>
+      <c r="D34" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>8</v>
@@ -1149,8 +1146,8 @@
       <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>7</v>
+      <c r="D35" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>8</v>
@@ -1166,8 +1163,8 @@
       <c r="C36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>38</v>
+      <c r="D36" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>8</v>
@@ -1183,8 +1180,8 @@
       <c r="C37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>38</v>
+      <c r="D37" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>8</v>
@@ -1200,8 +1197,8 @@
       <c r="C38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>7</v>
+      <c r="D38" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>8</v>
@@ -1217,8 +1214,8 @@
       <c r="C39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>38</v>
+      <c r="D39" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>8</v>
@@ -1234,8 +1231,8 @@
       <c r="C40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>7</v>
+      <c r="D40" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>8</v>

</xml_diff>